<commit_message>
Fixed id's for enrollment questionnaire
</commit_message>
<xml_diff>
--- a/vbai-fhir/ValueSet-fluent-language.xlsx
+++ b/vbai-fhir/ValueSet-fluent-language.xlsx
@@ -36,13 +36,13 @@
     <t>Name</t>
   </si>
   <si>
-    <t>EfFluentLanguage</t>
+    <t>FluentLanguage</t>
   </si>
   <si>
     <t>Title</t>
   </si>
   <si>
-    <t>Ef Fluent ValueSet</t>
+    <t>Fluent ValueSet</t>
   </si>
   <si>
     <t>Status</t>

</xml_diff>